<commit_message>
Last fixes from me
</commit_message>
<xml_diff>
--- a/henrar/results.xlsx
+++ b/henrar/results.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DRIVE\GIT\TPRLab3\henrar\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="20490" windowHeight="7890"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="20490" windowHeight="7890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Podstawowy" sheetId="1" r:id="rId1"/>
     <sheet name="Skalowalny" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>L. procesorów</t>
   </si>
@@ -42,11 +37,23 @@
   <si>
     <t>Procesory</t>
   </si>
+  <si>
+    <t>10^6</t>
+  </si>
+  <si>
+    <t>10^7</t>
+  </si>
+  <si>
+    <t>10^8</t>
+  </si>
+  <si>
+    <t>10^9</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;[$zł-415];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$zł-415]"/>
   </numFmts>
@@ -128,10 +135,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -150,14 +154,11 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -235,7 +236,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -314,7 +314,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -393,7 +392,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -461,25 +459,16 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="635386384"/>
-        <c:axId val="635397264"/>
+        <c:dLbls/>
+        <c:axId val="74680960"/>
+        <c:axId val="74679040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="635397264"/>
+        <c:axId val="74679040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -507,11 +496,9 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -527,19 +514,18 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="635386384"/>
+        <c:crossAx val="74680960"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="635386384"/>
+        <c:axId val="74680960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -558,11 +544,9 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -578,10 +562,10 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="635397264"/>
+        <c:crossAx val="74679040"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -598,7 +582,6 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -612,13 +595,12 @@
           <a:pPr>
             <a:defRPr sz="1000" b="0"/>
           </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln>
@@ -627,7 +609,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -635,10 +617,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -657,14 +636,11 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -742,7 +718,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -821,7 +796,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -900,7 +874,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -968,25 +941,16 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="686121184"/>
-        <c:axId val="686132064"/>
+        <c:dLbls/>
+        <c:axId val="47686400"/>
+        <c:axId val="47667840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="686132064"/>
+        <c:axId val="47667840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1014,11 +978,9 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -1034,19 +996,18 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="686121184"/>
+        <c:crossAx val="47686400"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="686121184"/>
+        <c:axId val="47686400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1065,11 +1026,9 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -1085,10 +1044,10 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="686132064"/>
+        <c:crossAx val="47667840"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1105,7 +1064,6 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1119,13 +1077,12 @@
           <a:pPr>
             <a:defRPr sz="1000" b="0"/>
           </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln>
@@ -1134,7 +1091,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1142,10 +1099,7 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1164,14 +1118,11 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1246,7 +1197,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1322,7 +1272,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1398,7 +1347,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1463,25 +1411,16 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="686135872"/>
-        <c:axId val="686124992"/>
+        <c:dLbls/>
+        <c:axId val="47733376"/>
+        <c:axId val="47731456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="686124992"/>
+        <c:axId val="47731456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1509,11 +1448,9 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -1529,19 +1466,18 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="686135872"/>
+        <c:crossAx val="47733376"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="686135872"/>
+        <c:axId val="47733376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1560,11 +1496,9 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -1580,10 +1514,10 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="686124992"/>
+        <c:crossAx val="47731456"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1600,7 +1534,6 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1614,13 +1547,12 @@
           <a:pPr>
             <a:defRPr sz="1000" b="0"/>
           </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln>
@@ -1629,7 +1561,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1637,10 +1569,7 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1659,14 +1588,11 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1744,7 +1670,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1823,7 +1748,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1902,7 +1826,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1970,25 +1893,16 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="686123360"/>
-        <c:axId val="686122272"/>
+        <c:dLbls/>
+        <c:axId val="47928448"/>
+        <c:axId val="47836160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="686122272"/>
+        <c:axId val="47836160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2016,11 +1930,9 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -2036,19 +1948,18 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="686123360"/>
+        <c:crossAx val="47928448"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="686123360"/>
+        <c:axId val="47928448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2067,11 +1978,9 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -2087,10 +1996,10 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="686122272"/>
+        <c:crossAx val="47836160"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2107,7 +2016,6 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2121,13 +2029,12 @@
           <a:pPr>
             <a:defRPr sz="1000" b="0"/>
           </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln>
@@ -2136,7 +2043,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2144,10 +2051,7 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2166,14 +2070,11 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2251,7 +2152,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2327,7 +2227,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2406,7 +2305,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -2474,25 +2372,16 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="686128256"/>
-        <c:axId val="686131520"/>
+        <c:dLbls/>
+        <c:axId val="47963136"/>
+        <c:axId val="47961216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="686131520"/>
+        <c:axId val="47961216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -2520,11 +2409,9 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -2540,19 +2427,18 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="686128256"/>
+        <c:crossAx val="47963136"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="686128256"/>
+        <c:axId val="47963136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2571,11 +2457,9 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -2591,10 +2475,10 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="686131520"/>
+        <c:crossAx val="47961216"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2611,7 +2495,6 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2625,13 +2508,12 @@
           <a:pPr>
             <a:defRPr sz="1000" b="0"/>
           </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln>
@@ -2640,7 +2522,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2648,10 +2530,7 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2670,14 +2549,11 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2752,7 +2628,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2828,7 +2703,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2904,7 +2778,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -2969,25 +2842,16 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="686134240"/>
-        <c:axId val="686133696"/>
+        <c:dLbls/>
+        <c:axId val="48116864"/>
+        <c:axId val="48110592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="686133696"/>
+        <c:axId val="48110592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -3015,11 +2879,9 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -3035,19 +2897,18 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="686134240"/>
+        <c:crossAx val="48116864"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="686134240"/>
+        <c:axId val="48116864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -3066,11 +2927,9 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
@@ -3086,10 +2945,10 @@
             <a:pPr>
               <a:defRPr sz="1000" b="0"/>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="686133696"/>
+        <c:crossAx val="48110592"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3106,7 +2965,6 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -3120,13 +2978,12 @@
           <a:pPr>
             <a:defRPr sz="1000" b="0"/>
           </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln>
@@ -3135,7 +2992,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3344,7 +3201,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3379,7 +3236,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3556,18 +3413,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3608,6 +3465,9 @@
       <c r="C2">
         <v>9.2658000000000004E-2</v>
       </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
       <c r="E2">
         <f>C2/C2</f>
         <v>1</v>
@@ -3765,6 +3625,9 @@
       <c r="C10">
         <v>0.58558600000000005</v>
       </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
       <c r="E10">
         <f>C10/C10</f>
         <v>1</v>
@@ -3922,6 +3785,9 @@
       <c r="C18">
         <v>5.4313269999999996</v>
       </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
       <c r="E18">
         <f>C18/C18</f>
         <v>1</v>
@@ -4078,6 +3944,9 @@
       </c>
       <c r="C26">
         <v>53.837656000000003</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
       </c>
       <c r="E26">
         <f>C26/C26</f>
@@ -4237,11 +4106,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4282,6 +4151,9 @@
       <c r="C2">
         <v>6.2488000000000002E-2</v>
       </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
       <c r="E2">
         <f>C2/C2</f>
         <v>1</v>

</xml_diff>